<commit_message>
Updated data, and ameliorated templates
</commit_message>
<xml_diff>
--- a/data/Loreal.xlsx
+++ b/data/Loreal.xlsx
@@ -9,19 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7440" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7440"/>
   </bookViews>
   <sheets>
     <sheet name="20 02 2017" sheetId="3" r:id="rId1"/>
     <sheet name="21 02 2017" sheetId="2" r:id="rId2"/>
     <sheet name="22 02 2017" sheetId="1" r:id="rId3"/>
+    <sheet name="23 02 2017" sheetId="4" r:id="rId4"/>
+    <sheet name="24 02 2017" sheetId="5" r:id="rId5"/>
+    <sheet name="27 02 2017" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="64">
   <si>
     <t>Critère</t>
   </si>
@@ -222,10 +225,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>j &lt; 0</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>M</t>
     </r>
@@ -267,12 +266,174 @@
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>Reason</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Score</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ignal crosse au dessus de MACD</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>A5 croisse au dessus de MA20</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ours entre bSup et bInf</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Final Score</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Score</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Score</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>A5 croisse au dessus de MA20</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reason</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>16h30</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Final Score</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>11h40</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cours superieur de bSup</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>k croisse au dessus de d</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Signal croisse au dessus de MACD</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSI proche de 70</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>11h30</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cours inferieur de bInf</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MA5  au dessous de MA20.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Signal decent au dessus de MACD</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSI &lt; 30, survente possible</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>k, d sont bas depuis longtemps. Meme s'il sont inferieur de 20 depuis 30 minutes, le cours pourrait continuer de decendre.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>j &lt; 0</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSI proche de 70</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ien</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>k croisse au dessus de d</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -321,6 +482,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -351,10 +518,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -379,9 +547,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -695,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -738,7 +920,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="6">
         <f ca="1">SUM(D2:D5)</f>
-        <v>6.8750000000000006E-2</v>
+        <v>1.7849999999999991E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -750,11 +932,11 @@
       </c>
       <c r="C3" s="6">
         <f>SUM(D11:D15)</f>
-        <v>0.35000000000000003</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D3" s="6">
         <f t="shared" si="0"/>
-        <v>7.8750000000000014E-2</v>
+        <v>6.5250000000000002E-2</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -790,11 +972,11 @@
       </c>
       <c r="C5" s="6">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.44</v>
+        <v>-0.66</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>-7.4800000000000005E-2</v>
+        <v>-0.11220000000000001</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -883,14 +1065,14 @@
         <v>0.2</v>
       </c>
       <c r="C12" s="5">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="D12" s="6">
         <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>28</v>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1108,7 +1290,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1150,7 +1332,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="6">
         <f ca="1">SUM(D2:D5)</f>
-        <v>9.8050000000000026E-2</v>
+        <v>0.12355000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1202,11 +1384,11 @@
       </c>
       <c r="C5" s="6">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.4</v>
+        <v>-0.25</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.8000000000000005E-2</v>
+        <v>-4.2500000000000003E-2</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1519,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1562,7 +1744,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="6">
         <f ca="1">SUM(D2:D5)</f>
-        <v>-9.0900000000000009E-2</v>
+        <v>-3.3999999999999989E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1574,11 +1756,11 @@
       </c>
       <c r="C3" s="6">
         <f>SUM(D11:D15)</f>
-        <v>-8.0000000000000016E-2</v>
+        <v>0.12</v>
       </c>
       <c r="D3" s="6">
         <f t="shared" si="0"/>
-        <v>-1.8000000000000006E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -1614,11 +1796,11 @@
       </c>
       <c r="C5" s="6">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.81</v>
+        <v>-0.74</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.13770000000000002</v>
+        <v>-0.1258</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1707,14 +1889,14 @@
         <v>0.2</v>
       </c>
       <c r="C12" s="5">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="6">
         <f t="shared" si="1"/>
-        <v>-0.2</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>33</v>
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1734,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1754,7 +1936,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1774,7 +1956,7 @@
         <v>0.06</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1925,4 +2107,1234 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="14.42578125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="20">
+        <v>0.38</v>
+      </c>
+      <c r="C2" s="19">
+        <v>0</v>
+      </c>
+      <c r="D2" s="16">
+        <f>B2*C2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16">
+        <f ca="1">SUM(D2:D5)</f>
+        <v>0.21810000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="16">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C3" s="16">
+        <f>SUM(D11:D15)</f>
+        <v>0.84</v>
+      </c>
+      <c r="D3" s="16">
+        <f>B3*C3</f>
+        <v>0.189</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C4" s="16">
+        <f>SUM(D20:D24)</f>
+        <v>0.28800000000000003</v>
+      </c>
+      <c r="D4" s="16">
+        <f>B4*C4</f>
+        <v>6.480000000000001E-2</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="16">
+        <v>0.17</v>
+      </c>
+      <c r="C5" s="16">
+        <f ca="1">RANDBETWEEN(-100,100) / 100</f>
+        <v>-0.21</v>
+      </c>
+      <c r="D5" s="16">
+        <f ca="1">B5*C5</f>
+        <v>-3.5700000000000003E-2</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C11" s="19">
+        <v>1</v>
+      </c>
+      <c r="D11" s="16">
+        <f>B11*C11</f>
+        <v>0.2</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C12" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="D12" s="16">
+        <f>B12*C12</f>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C13" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="D13" s="16">
+        <f>B13*C13</f>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C14" s="19">
+        <v>1</v>
+      </c>
+      <c r="D14" s="16">
+        <f>B14*C14</f>
+        <v>0.2</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C15" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="D15" s="16">
+        <f>B15*C15</f>
+        <v>0.12</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C20" s="8">
+        <v>-0.04</v>
+      </c>
+      <c r="D20" s="6">
+        <f t="shared" ref="D20:D24" si="0">B20*C20</f>
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0.52</v>
+      </c>
+      <c r="D21" s="6">
+        <f t="shared" si="0"/>
+        <v>0.10400000000000001</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.52</v>
+      </c>
+      <c r="D22" s="6">
+        <f t="shared" si="0"/>
+        <v>0.10400000000000001</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="D23" s="6">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0.24</v>
+      </c>
+      <c r="D24" s="6">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="14.42578125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="20">
+        <v>0.38</v>
+      </c>
+      <c r="C2" s="19">
+        <v>0</v>
+      </c>
+      <c r="D2" s="16">
+        <f>B2*C2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16">
+        <f ca="1">SUM(D2:D5)</f>
+        <v>6.2300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="16">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C3" s="16">
+        <f>SUM(D11:D15)</f>
+        <v>-0.20000000000000004</v>
+      </c>
+      <c r="D3" s="16">
+        <f>B3*C3</f>
+        <v>-4.5000000000000012E-2</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C4" s="16">
+        <f>SUM(D20:D24)</f>
+        <v>0.28800000000000003</v>
+      </c>
+      <c r="D4" s="16">
+        <f>B4*C4</f>
+        <v>6.480000000000001E-2</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="16">
+        <v>0.17</v>
+      </c>
+      <c r="C5" s="16">
+        <f ca="1">RANDBETWEEN(-100,100) / 100</f>
+        <v>0.25</v>
+      </c>
+      <c r="D5" s="16">
+        <f ca="1">B5*C5</f>
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C11" s="19">
+        <v>-1</v>
+      </c>
+      <c r="D11" s="16">
+        <f>B11*C11</f>
+        <v>-0.2</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C12" s="19">
+        <v>0</v>
+      </c>
+      <c r="D12" s="16">
+        <f>B12*C12</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C13" s="19">
+        <v>-0.5</v>
+      </c>
+      <c r="D13" s="16">
+        <f>B13*C13</f>
+        <v>-0.1</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C14" s="19">
+        <v>0</v>
+      </c>
+      <c r="D14" s="16">
+        <f>B14*C14</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C15" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="16">
+        <f>B15*C15</f>
+        <v>0.1</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C20" s="8">
+        <v>-0.04</v>
+      </c>
+      <c r="D20" s="6">
+        <f t="shared" ref="D20:D24" si="0">B20*C20</f>
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0.52</v>
+      </c>
+      <c r="D21" s="6">
+        <f t="shared" si="0"/>
+        <v>0.10400000000000001</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.52</v>
+      </c>
+      <c r="D22" s="6">
+        <f t="shared" si="0"/>
+        <v>0.10400000000000001</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="D23" s="6">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0.24</v>
+      </c>
+      <c r="D24" s="6">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="14.42578125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="20">
+        <v>0.38</v>
+      </c>
+      <c r="C2" s="19">
+        <v>0</v>
+      </c>
+      <c r="D2" s="16">
+        <f>B2*C2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16">
+        <f ca="1">SUM(D2:D5)</f>
+        <v>8.6300000000000043E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="16">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C3" s="16">
+        <f>SUM(D11:D15)</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="D3" s="16">
+        <f>B3*C3</f>
+        <v>0.15750000000000003</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C4" s="16">
+        <f>SUM(D20:D24)</f>
+        <v>0.28800000000000003</v>
+      </c>
+      <c r="D4" s="16">
+        <f>B4*C4</f>
+        <v>6.480000000000001E-2</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="16">
+        <v>0.17</v>
+      </c>
+      <c r="C5" s="16">
+        <f ca="1">RANDBETWEEN(-100,100) / 100</f>
+        <v>-0.8</v>
+      </c>
+      <c r="D5" s="16">
+        <f ca="1">B5*C5</f>
+        <v>-0.13600000000000001</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C11" s="19">
+        <v>0</v>
+      </c>
+      <c r="D11" s="16">
+        <f>B11*C11</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C12" s="19">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16">
+        <f>B12*C12</f>
+        <v>0.2</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C13" s="19">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16">
+        <f>B13*C13</f>
+        <v>0.2</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C14" s="19">
+        <v>1</v>
+      </c>
+      <c r="D14" s="16">
+        <f>B14*C14</f>
+        <v>0.2</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C15" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="16">
+        <f>B15*C15</f>
+        <v>0.1</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C20" s="8">
+        <v>-0.04</v>
+      </c>
+      <c r="D20" s="6">
+        <f t="shared" ref="D20:D24" si="0">B20*C20</f>
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0.52</v>
+      </c>
+      <c r="D21" s="6">
+        <f t="shared" si="0"/>
+        <v>0.10400000000000001</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.52</v>
+      </c>
+      <c r="D22" s="6">
+        <f t="shared" si="0"/>
+        <v>0.10400000000000001</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="D23" s="6">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0.24</v>
+      </c>
+      <c r="D24" s="6">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Airbus and Biomerieux datas
</commit_message>
<xml_diff>
--- a/data/Loreal.xlsx
+++ b/data/Loreal.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7440" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="20 02 2017" sheetId="3" r:id="rId1"/>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -920,7 +920,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="6">
         <f ca="1">SUM(D2:D5)</f>
-        <v>1.7849999999999991E-2</v>
+        <v>-1.7850000000000005E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -972,11 +972,11 @@
       </c>
       <c r="C5" s="6">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.66</v>
+        <v>-0.87</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.11220000000000001</v>
+        <v>-0.1479</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1332,7 +1332,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="6">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.12355000000000002</v>
+        <v>0.10145000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1384,11 +1384,11 @@
       </c>
       <c r="C5" s="6">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.25</v>
+        <v>-0.38</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.2500000000000003E-2</v>
+        <v>-6.4600000000000005E-2</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1744,7 +1744,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="6">
         <f ca="1">SUM(D2:D5)</f>
-        <v>-3.3999999999999989E-2</v>
+        <v>0.12580000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1796,11 +1796,11 @@
       </c>
       <c r="C5" s="6">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.74</v>
+        <v>0.2</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.1258</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -2159,7 +2159,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="16">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.21810000000000002</v>
+        <v>9.7400000000000014E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2211,11 +2211,11 @@
       </c>
       <c r="C5" s="16">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.21</v>
+        <v>-0.92</v>
       </c>
       <c r="D5" s="16">
         <f ca="1">B5*C5</f>
-        <v>-3.5700000000000003E-2</v>
+        <v>-0.15640000000000001</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -2569,7 +2569,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="16">
         <f ca="1">SUM(D2:D5)</f>
-        <v>6.2300000000000001E-2</v>
+        <v>-1.4200000000000004E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2621,11 +2621,11 @@
       </c>
       <c r="C5" s="16">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.25</v>
+        <v>-0.2</v>
       </c>
       <c r="D5" s="16">
         <f ca="1">B5*C5</f>
-        <v>4.2500000000000003E-2</v>
+        <v>-3.4000000000000002E-2</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -2933,13 +2933,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="14.42578125" style="14"/>
+    <col min="1" max="1" width="21.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="14.42578125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2979,7 +2980,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="16">
         <f ca="1">SUM(D2:D5)</f>
-        <v>8.6300000000000043E-2</v>
+        <v>0.23250000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3031,11 +3032,11 @@
       </c>
       <c r="C5" s="16">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.8</v>
+        <v>0.06</v>
       </c>
       <c r="D5" s="16">
         <f ca="1">B5*C5</f>
-        <v>-0.13600000000000001</v>
+        <v>1.0200000000000001E-2</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>

</xml_diff>

<commit_message>
oreal finance score fixed
</commit_message>
<xml_diff>
--- a/data/Loreal.xlsx
+++ b/data/Loreal.xlsx
@@ -990,7 +990,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>-1.2750000000000011E-2</v>
+        <v>0.25414999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1042,11 +1042,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.84</v>
+        <v>0.73</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>-0.14280000000000001</v>
+        <v>0.1241</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -1418,7 +1418,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.48600000000000004</v>
+        <v>0.25990000000000002</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -1527,11 +1527,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.96</v>
+        <v>-0.37</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>0.16320000000000001</v>
+        <v>-6.2899999999999998E-2</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -2284,7 +2284,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.44230000000000003</v>
+        <v>0.31310000000000004</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -2393,11 +2393,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.65</v>
+        <v>-0.11</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>0.11050000000000001</v>
+        <v>-1.8700000000000001E-2</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -3150,7 +3150,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>-0.10819999999999999</v>
+        <v>-9.8000000000000004E-2</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -3259,11 +3259,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.7</v>
+        <v>-0.64</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>-0.11899999999999999</v>
+        <v>-0.10880000000000001</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -3953,7 +3953,7 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C20" sqref="C20:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4018,7 +4018,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.44950000000000001</v>
+        <v>0.26080000000000003</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -4127,11 +4127,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.86</v>
+        <v>-0.25</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>0.1462</v>
+        <v>-4.2500000000000003E-2</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -4820,7 +4820,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C20" sqref="C20:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4866,7 +4866,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>-0.1173</v>
+        <v>0.14810000000000001</v>
       </c>
       <c r="H2" s="11"/>
     </row>
@@ -4901,11 +4901,11 @@
       </c>
       <c r="C4" s="5">
         <f>SUM(D20:D24)</f>
-        <v>0</v>
+        <v>0.28800000000000003</v>
       </c>
       <c r="D4" s="5">
         <f>B4*C4</f>
-        <v>0</v>
+        <v>6.480000000000001E-2</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -4921,11 +4921,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.69</v>
+        <v>0.49</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>-0.1173</v>
+        <v>8.3299999999999999E-2</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -5144,11 +5144,11 @@
         <v>0.2</v>
       </c>
       <c r="C20" s="8">
-        <v>0</v>
+        <v>-0.04</v>
       </c>
       <c r="D20" s="5">
         <f>B20*C20</f>
-        <v>0</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -5163,11 +5163,11 @@
         <v>0.2</v>
       </c>
       <c r="C21" s="8">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="D21" s="5">
         <f>B21*C21</f>
-        <v>0</v>
+        <v>0.10400000000000001</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -5182,11 +5182,11 @@
         <v>0.2</v>
       </c>
       <c r="C22" s="9">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="D22" s="5">
         <f>B22*C22</f>
-        <v>0</v>
+        <v>0.10400000000000001</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -5201,11 +5201,11 @@
         <v>0.2</v>
       </c>
       <c r="C23" s="9">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D23" s="5">
         <f>B23*C23</f>
-        <v>0</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -5220,11 +5220,11 @@
         <v>0.2</v>
       </c>
       <c r="C24" s="9">
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="D24" s="5">
         <f>B24*C24</f>
-        <v>0</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -5243,7 +5243,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C20" sqref="C20:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5289,7 +5289,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.1207</v>
+        <v>0.20930000000000004</v>
       </c>
       <c r="H2" s="14"/>
     </row>
@@ -5324,11 +5324,11 @@
       </c>
       <c r="C4" s="5">
         <f>SUM(D20:D24)</f>
-        <v>0</v>
+        <v>0.28800000000000003</v>
       </c>
       <c r="D4" s="5">
         <f>B4*C4</f>
-        <v>0</v>
+        <v>6.480000000000001E-2</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -5344,11 +5344,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.71</v>
+        <v>0.85</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>0.1207</v>
+        <v>0.14450000000000002</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -5567,11 +5567,11 @@
         <v>0.2</v>
       </c>
       <c r="C20" s="8">
-        <v>0</v>
+        <v>-0.04</v>
       </c>
       <c r="D20" s="5">
         <f>B20*C20</f>
-        <v>0</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -5586,11 +5586,11 @@
         <v>0.2</v>
       </c>
       <c r="C21" s="8">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="D21" s="5">
         <f>B21*C21</f>
-        <v>0</v>
+        <v>0.10400000000000001</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -5605,11 +5605,11 @@
         <v>0.2</v>
       </c>
       <c r="C22" s="9">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="D22" s="5">
         <f>B22*C22</f>
-        <v>0</v>
+        <v>0.10400000000000001</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -5624,11 +5624,11 @@
         <v>0.2</v>
       </c>
       <c r="C23" s="9">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D23" s="5">
         <f>B23*C23</f>
-        <v>0</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -5643,11 +5643,11 @@
         <v>0.2</v>
       </c>
       <c r="C24" s="9">
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="D24" s="5">
         <f>B24*C24</f>
-        <v>0</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -5666,7 +5666,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C20" sqref="C20:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5712,7 +5712,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>2.7200000000000002E-2</v>
+        <v>0.13280000000000003</v>
       </c>
       <c r="H2" s="14"/>
     </row>
@@ -5747,11 +5747,11 @@
       </c>
       <c r="C4" s="5">
         <f>SUM(D20:D24)</f>
-        <v>0</v>
+        <v>0.28800000000000003</v>
       </c>
       <c r="D4" s="5">
         <f>B4*C4</f>
-        <v>0</v>
+        <v>6.480000000000001E-2</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -5767,11 +5767,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.16</v>
+        <v>0.4</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>2.7200000000000002E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -5990,11 +5990,11 @@
         <v>0.2</v>
       </c>
       <c r="C20" s="8">
-        <v>0</v>
+        <v>-0.04</v>
       </c>
       <c r="D20" s="5">
         <f>B20*C20</f>
-        <v>0</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -6009,11 +6009,11 @@
         <v>0.2</v>
       </c>
       <c r="C21" s="8">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="D21" s="5">
         <f>B21*C21</f>
-        <v>0</v>
+        <v>0.10400000000000001</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -6028,11 +6028,11 @@
         <v>0.2</v>
       </c>
       <c r="C22" s="9">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="D22" s="5">
         <f>B22*C22</f>
-        <v>0</v>
+        <v>0.10400000000000001</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -6047,11 +6047,11 @@
         <v>0.2</v>
       </c>
       <c r="C23" s="9">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D23" s="5">
         <f>B23*C23</f>
-        <v>0</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -6066,11 +6066,11 @@
         <v>0.2</v>
       </c>
       <c r="C24" s="9">
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="D24" s="5">
         <f>B24*C24</f>
-        <v>0</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -6089,7 +6089,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C20" sqref="C20:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6135,7 +6135,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.16320000000000001</v>
+        <v>-6.0999999999999985E-2</v>
       </c>
       <c r="H2" s="14"/>
     </row>
@@ -6170,11 +6170,11 @@
       </c>
       <c r="C4" s="5">
         <f>SUM(D20:D24)</f>
-        <v>0</v>
+        <v>0.28800000000000003</v>
       </c>
       <c r="D4" s="5">
         <f>B4*C4</f>
-        <v>0</v>
+        <v>6.480000000000001E-2</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -6190,11 +6190,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.96</v>
+        <v>-0.74</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>0.16320000000000001</v>
+        <v>-0.1258</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -6413,11 +6413,11 @@
         <v>0.2</v>
       </c>
       <c r="C20" s="8">
-        <v>0</v>
+        <v>-0.04</v>
       </c>
       <c r="D20" s="5">
         <f>B20*C20</f>
-        <v>0</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -6432,11 +6432,11 @@
         <v>0.2</v>
       </c>
       <c r="C21" s="8">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="D21" s="5">
         <f>B21*C21</f>
-        <v>0</v>
+        <v>0.10400000000000001</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -6451,11 +6451,11 @@
         <v>0.2</v>
       </c>
       <c r="C22" s="9">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="D22" s="5">
         <f>B22*C22</f>
-        <v>0</v>
+        <v>0.10400000000000001</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -6470,11 +6470,11 @@
         <v>0.2</v>
       </c>
       <c r="C23" s="9">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D23" s="5">
         <f>B23*C23</f>
-        <v>0</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -6489,11 +6489,11 @@
         <v>0.2</v>
       </c>
       <c r="C24" s="9">
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="D24" s="5">
         <f>B24*C24</f>
-        <v>0</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -6512,7 +6512,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C20" sqref="C20:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6558,7 +6558,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>1.7000000000000001E-3</v>
+        <v>-7.2900000000000006E-2</v>
       </c>
       <c r="H2" s="14"/>
     </row>
@@ -6593,11 +6593,11 @@
       </c>
       <c r="C4" s="5">
         <f>SUM(D20:D24)</f>
-        <v>0</v>
+        <v>0.28800000000000003</v>
       </c>
       <c r="D4" s="5">
         <f>B4*C4</f>
-        <v>0</v>
+        <v>6.480000000000001E-2</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -6613,11 +6613,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.01</v>
+        <v>-0.81</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>1.7000000000000001E-3</v>
+        <v>-0.13770000000000002</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -6836,11 +6836,11 @@
         <v>0.2</v>
       </c>
       <c r="C20" s="8">
-        <v>0</v>
+        <v>-0.04</v>
       </c>
       <c r="D20" s="5">
         <f>B20*C20</f>
-        <v>0</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -6855,11 +6855,11 @@
         <v>0.2</v>
       </c>
       <c r="C21" s="8">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="D21" s="5">
         <f>B21*C21</f>
-        <v>0</v>
+        <v>0.10400000000000001</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -6874,11 +6874,11 @@
         <v>0.2</v>
       </c>
       <c r="C22" s="9">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="D22" s="5">
         <f>B22*C22</f>
-        <v>0</v>
+        <v>0.10400000000000001</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -6893,11 +6893,11 @@
         <v>0.2</v>
       </c>
       <c r="C23" s="9">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D23" s="5">
         <f>B23*C23</f>
-        <v>0</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -6912,11 +6912,11 @@
         <v>0.2</v>
       </c>
       <c r="C24" s="9">
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="D24" s="5">
         <f>B24*C24</f>
-        <v>0</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -6979,7 +6979,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>6.5750000000000031E-2</v>
+        <v>0.12525000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -7031,11 +7031,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.59</v>
+        <v>-0.24</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>-0.1003</v>
+        <v>-4.0800000000000003E-2</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -7388,7 +7388,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.25840000000000002</v>
+        <v>-6.7999999999999991E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -7440,11 +7440,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.98</v>
+        <v>-0.94</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>0.1666</v>
+        <v>-0.1598</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -7816,7 +7816,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.19260000000000002</v>
+        <v>9.4000000000000028E-2</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -7925,11 +7925,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.36</v>
+        <v>-0.94</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>-6.1200000000000004E-2</v>
+        <v>-0.1598</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -8681,7 +8681,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>1.9799999999999998E-2</v>
+        <v>0.15579999999999999</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -8790,11 +8790,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>0</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -9547,7 +9547,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.24100000000000005</v>
+        <v>0.32940000000000008</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -9656,11 +9656,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.11</v>
+        <v>0.63</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>1.8700000000000001E-2</v>
+        <v>0.10710000000000001</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -10412,7 +10412,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>9.2500000000000054E-2</v>
+        <v>0.19620000000000004</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -10521,11 +10521,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.79</v>
+        <v>-0.18</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>-0.1343</v>
+        <v>-3.0600000000000002E-2</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -11206,7 +11206,7 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11278,7 +11278,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>3.5300000000000012E-2</v>
+        <v>0.21040000000000003</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -11387,11 +11387,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.2</v>
+        <v>0.83</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>-3.4000000000000002E-2</v>
+        <v>0.1411</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -12144,7 +12144,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5">
         <f ca="1">SUM(D2:D5)</f>
-        <v>5.7900000000000007E-2</v>
+        <v>-6.9599999999999995E-2</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -12253,11 +12253,11 @@
       </c>
       <c r="C5" s="5">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.12</v>
+        <v>-0.87</v>
       </c>
       <c r="D5" s="5">
         <f ca="1">B5*C5</f>
-        <v>-2.0400000000000001E-2</v>
+        <v>-0.1479</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>

</xml_diff>